<commit_message>
feat: added jwt sessions and lots of graphql queries
</commit_message>
<xml_diff>
--- a/docs/db-design.xlsx
+++ b/docs/db-design.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="33">
   <si>
     <t xml:space="preserve">stories</t>
   </si>
@@ -88,13 +88,7 @@
     <t xml:space="preserve">scene_descriptions</t>
   </si>
   <si>
-    <t xml:space="preserve">session_token</t>
-  </si>
-  <si>
-    <t xml:space="preserve">session_expiry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INTEGER</t>
+    <t xml:space="preserve">session</t>
   </si>
   <si>
     <t xml:space="preserve">progress</t>
@@ -139,6 +133,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -160,6 +155,7 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="8">
@@ -259,87 +255,87 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -423,157 +419,153 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="E1" s="3" t="s">
+      <c r="B1" s="3"/>
+      <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="8" t="s">
+      <c r="F3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="10"/>
+      <c r="B4" s="11"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="13" t="s">
+      <c r="F6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="8" t="s">
+      <c r="F7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="4"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="7" t="s">
+      <c r="F10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="5" t="s">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="E11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="7" t="s">
         <v>5</v>
       </c>
       <c r="G11" s="14" t="s">
@@ -581,11 +573,11 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E12" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>26</v>
+      <c r="E12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -593,41 +585,41 @@
         <v>6</v>
       </c>
       <c r="B13" s="16"/>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E16" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" s="7" t="s">
+      <c r="F16" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="8" t="s">
         <v>6</v>
       </c>
     </row>
@@ -636,78 +628,78 @@
         <v>14</v>
       </c>
       <c r="B17" s="18"/>
-      <c r="E17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G17" s="7" t="s">
+      <c r="E17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="6" t="s">
+      <c r="E18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="12" t="s">
+      <c r="A19" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="6" t="s">
+      <c r="E19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="12" t="s">
+      <c r="A20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="7" t="s">
+      <c r="B21" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="4"/>
+      <c r="E21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G22" s="13" t="s">
+      <c r="F22" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="12" t="s">
         <v>14</v>
       </c>
     </row>
@@ -716,10 +708,10 @@
         <v>8</v>
       </c>
       <c r="B23" s="21"/>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F23" s="7" t="s">
         <v>5</v>
       </c>
       <c r="G23" s="14" t="s">
@@ -727,32 +719,32 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F24" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="7" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>